<commit_message>
Implemented importing dataroom structure from excel, project is Working now. But need some adjustments and error handling.
</commit_message>
<xml_diff>
--- a/potato.xlsx
+++ b/potato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moustaphabazzoun/Documents/CVProjects/DataRoom-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077B5E9C-553B-6241-9BB7-5A5D0F00A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB853C7-FECC-3B48-B096-A90C99EC09DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15720" xr2:uid="{BA023689-3E57-EB47-AFA4-2ADE842A1313}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Financials</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>CNPJ</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -455,83 +461,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6F95BC-55B9-884B-A68D-8B3E2CD158EC}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="1">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>